<commit_message>
AddOrder implemented.  Adding PlantUML diagram for state machine.  Creating helper sub-vi's for retrieving fields.  Rest of Order types should be implemented relatively quickly now.
</commit_message>
<xml_diff>
--- a/Field.Mappings.xlsx
+++ b/Field.Mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\arty_bats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\Arty\arty_bats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D14AF13-E4AD-4E2D-B015-097E4EAB4836}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744EAE44-9199-4C02-83B9-B2159CA7BE29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14AF859B-DC12-4D22-B03E-17433F3793C5}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{14AF859B-DC12-4D22-B03E-17433F3793C5}"/>
   </bookViews>
   <sheets>
     <sheet name="State Machine" sheetId="8" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="106">
   <si>
     <t>Add Order (long)</t>
   </si>
@@ -184,15 +184,6 @@
     <t>0x23</t>
   </si>
   <si>
-    <t>Keep?</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Sequenced Unit Header</t>
   </si>
   <si>
@@ -380,38 +371,14 @@
     <t>Order Id of a previously sent Add Order message that has completely been cancelled</t>
   </si>
   <si>
-    <t>Not now</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>counter</t>
-  </si>
-  <si>
-    <t>out</t>
-  </si>
-  <si>
-    <t>counter &lt;= counter +1</t>
-  </si>
-  <si>
-    <t>new_state &lt;= Read_Sequenced_Unit_Header</t>
-  </si>
-  <si>
-    <t>Read_Sequenced_Unit_Header</t>
+    <t>0x2f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,13 +395,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,11 +422,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -489,21 +468,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thick">
         <color indexed="64"/>
@@ -534,59 +498,9 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -601,17 +515,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thick">
@@ -783,21 +686,6 @@
     </border>
     <border>
       <left/>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
@@ -830,17 +718,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
@@ -1000,135 +877,308 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="39" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="49" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="47" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="45" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1440,53 +1490,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB48A11-9AF5-4678-A9D5-2A9EC9416E28}">
-  <dimension ref="A3:C9"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
@@ -1496,64 +1507,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB4D78B-89D3-4D42-8967-6C5C066C56EF}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="38" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="56"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="40">
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="27">
         <v>0</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="27">
         <v>2</v>
       </c>
-      <c r="D3" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="D3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -1564,13 +1575,13 @@
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E4" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
@@ -1581,30 +1592,30 @@
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="45" t="s">
+      <c r="E5" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="46">
+    </row>
+    <row r="6" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="33">
         <v>4</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="33">
         <v>4</v>
       </c>
-      <c r="D6" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="47" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E7" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1620,63 +1631,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6DC02A-D941-4271-B6A4-E0DAF8D23EE5}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.453125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="38" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="56"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="28" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="40">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27">
         <v>0</v>
       </c>
-      <c r="C3" s="40">
-        <v>1</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C3" s="27">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1687,32 +1698,32 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="33">
+        <v>2</v>
+      </c>
+      <c r="C5" s="33">
+        <v>4</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="46">
-        <v>2</v>
-      </c>
-      <c r="C5" s="46">
-        <v>4</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E6" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1725,109 +1736,106 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD1C4CA-5C90-4A34-878A-59E27B107822}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.81640625" customWidth="1"/>
-    <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.81640625" customWidth="1"/>
-    <col min="11" max="11" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.90625" customWidth="1"/>
-    <col min="13" max="13" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.81640625" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" customWidth="1"/>
+    <col min="13" max="13" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="66" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="62" t="s">
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="24" t="s">
+      <c r="L1" s="58"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="5"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="19" t="s">
+      <c r="H2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="37"/>
-    </row>
-    <row r="3" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1839,39 +1847,37 @@
       <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>0</v>
       </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3" s="12">
-        <v>1</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="34" t="s">
+      <c r="M3" s="11">
+        <v>1</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -1911,17 +1917,15 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -1966,16 +1970,16 @@
       <c r="O5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P5" s="36"/>
-    </row>
-    <row r="6" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="48" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="46">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1984,13 +1988,13 @@
       <c r="E6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="47" t="s">
         <v>4</v>
       </c>
       <c r="G6">
         <v>6</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="47">
         <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1999,13 +2003,13 @@
       <c r="J6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="47" t="s">
         <v>4</v>
       </c>
       <c r="L6">
         <v>6</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="47">
         <v>8</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -2014,18 +2018,16 @@
       <c r="O6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P6" s="36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="48" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>14</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="46">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2034,13 +2036,13 @@
       <c r="E7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="48" t="s">
         <v>5</v>
       </c>
       <c r="G7">
         <v>14</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="47">
         <v>1</v>
       </c>
       <c r="I7" t="s">
@@ -2049,13 +2051,13 @@
       <c r="J7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="47" t="s">
         <v>5</v>
       </c>
       <c r="L7">
         <v>14</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="47">
         <v>1</v>
       </c>
       <c r="N7" t="s">
@@ -2064,18 +2066,16 @@
       <c r="O7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P7" s="36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8">
         <v>15</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="50">
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -2084,13 +2084,13 @@
       <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8">
         <v>15</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="49">
         <v>2</v>
       </c>
       <c r="I8" t="s">
@@ -2099,33 +2099,30 @@
       <c r="J8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8">
         <v>15</v>
       </c>
-      <c r="M8" s="27">
+      <c r="M8" s="50">
         <v>4</v>
       </c>
       <c r="N8" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P8" s="36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A9" s="25" t="s">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9">
         <v>19</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="50">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -2134,13 +2131,13 @@
       <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9">
         <v>17</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="50">
         <v>6</v>
       </c>
       <c r="I9" t="s">
@@ -2149,48 +2146,45 @@
       <c r="J9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9">
         <v>19</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="50">
         <v>8</v>
       </c>
       <c r="N9" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P9" s="36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10">
         <v>25</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="50">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10">
         <v>23</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="49">
         <v>2</v>
       </c>
       <c r="I10" t="s">
@@ -2199,57 +2193,54 @@
       <c r="J10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10">
         <v>27</v>
       </c>
-      <c r="M10" s="27">
+      <c r="M10" s="50">
         <v>8</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P10" s="36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="13" t="s">
+    </row>
+    <row r="11" spans="1:16" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>33</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="14">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="1">
         <v>25</v>
       </c>
-      <c r="H11" s="16">
-        <v>1</v>
-      </c>
-      <c r="I11" s="16" t="s">
+      <c r="H11" s="14">
+        <v>1</v>
+      </c>
+      <c r="I11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" t="s">
         <v>9</v>
       </c>
       <c r="L11">
@@ -2261,50 +2252,55 @@
       <c r="N11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" ht="145.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="48" t="s">
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="144.6" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="J12" s="48" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="I12" t="str">
+        <f>DEC2HEX(26)</f>
+        <v>1A</v>
+      </c>
+      <c r="J12" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="28" t="s">
+      <c r="K12" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12">
         <v>36</v>
       </c>
-      <c r="M12" s="31">
+      <c r="M12">
         <v>4</v>
       </c>
       <c r="N12" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="P12" s="36"/>
-    </row>
-    <row r="13" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="K13" s="28" t="s">
+      <c r="I13">
+        <v>1921</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13">
         <v>40</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13">
         <v>1</v>
       </c>
       <c r="N13" t="s">
@@ -2313,31 +2309,31 @@
       <c r="O13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="36"/>
-    </row>
-    <row r="14" spans="1:17" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="K14" s="32" t="s">
+      <c r="K14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L14" s="33">
+      <c r="L14" s="14">
         <v>41</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M14" s="14">
         <v>4</v>
       </c>
-      <c r="N14" s="16" t="s">
+      <c r="N14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="O14" s="35" t="s">
+      <c r="O14" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="P14" s="37"/>
-    </row>
-    <row r="15" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="O15" s="4" t="s">
         <v>39</v>
       </c>
@@ -2357,102 +2353,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B73E5EA-889B-4BE9-9F66-5BFE749E4DE6}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="5" max="5" width="28.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.90625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="51" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="C2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="37" t="s">
+      <c r="H2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12">
+    <row r="3" spans="1:11" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="34" t="s">
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12">
+      <c r="F3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11">
         <v>0</v>
       </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="56" t="s">
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="42" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2466,7 +2462,7 @@
         <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>2</v>
@@ -2478,16 +2474,14 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2519,191 +2513,181 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="49" t="s">
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="46">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="45" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
         <v>6</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="46">
         <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>61</v>
       </c>
       <c r="B7" s="1">
         <v>14</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="46">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>61</v>
       </c>
       <c r="G7" s="1">
         <v>14</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="46">
         <v>4</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
+        <v>62</v>
       </c>
       <c r="B8" s="1">
         <v>18</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="46">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="49" t="s">
-        <v>74</v>
+        <v>67</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>71</v>
       </c>
       <c r="G8" s="1">
         <v>18</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="49">
         <v>4</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="16">
+        <v>73</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="14">
         <v>26</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="54">
+        <v>68</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="40">
         <v>22</v>
       </c>
-      <c r="H9" s="54">
+      <c r="H9" s="46">
         <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="12"/>
-      <c r="E10" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="11"/>
+      <c r="E10" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G10" s="40">
         <v>30</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="46">
         <v>8</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="40" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E11" s="2"/>
-      <c r="F11" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="46">
+      <c r="F11" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="33">
         <v>38</v>
       </c>
-      <c r="H11" s="46">
-        <v>1</v>
-      </c>
-      <c r="I11" s="46" t="s">
+      <c r="H11" s="33">
+        <v>1</v>
+      </c>
+      <c r="I11" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="J12" s="57" t="s">
-        <v>79</v>
+      <c r="J11" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="39" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2720,102 +2704,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521C613D-E1BF-4F72-83CC-60E44600563A}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="5" max="5" width="28.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.90625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="64" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="51" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="C2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="37" t="s">
+      <c r="H2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12">
+    <row r="3" spans="1:11" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="34" t="s">
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12">
+      <c r="F3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11">
         <v>0</v>
       </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="56" t="s">
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="42" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2826,10 +2810,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>2</v>
@@ -2841,16 +2825,14 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2882,91 +2864,87 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="49" t="s">
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="46">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="46" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
         <v>6</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="46">
         <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="16">
-        <v>14</v>
-      </c>
-      <c r="C7" s="16">
+        <v>85</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="14">
+        <v>14</v>
+      </c>
+      <c r="C7" s="52">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="58">
-        <v>14</v>
-      </c>
-      <c r="H7" s="58">
+        <v>86</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="44">
+        <v>14</v>
+      </c>
+      <c r="H7" s="53">
         <v>2</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="12"/>
-      <c r="E8" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="12"/>
+      <c r="I7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="11"/>
+      <c r="E8" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="11"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="48" t="s">
-        <v>79</v>
+      <c r="J8" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2989,101 +2967,101 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="5" max="5" width="28.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.90625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="65"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="51" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="C2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="37" t="s">
+      <c r="H2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12">
+    <row r="3" spans="1:11" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="34" t="s">
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12">
-        <v>1</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="56" t="s">
+      <c r="F3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="11">
+        <v>1</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="42" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3094,10 +3072,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>2</v>
@@ -3108,17 +3086,15 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3128,7 +3104,7 @@
       <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="40" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -3143,7 +3119,7 @@
       <c r="H5">
         <v>4</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="40" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="6" t="s">
@@ -3151,159 +3127,153 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="49" t="s">
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="46">
         <v>8</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="40" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="46" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
         <v>6</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="47">
         <v>8</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="40" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>14</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="46">
         <v>4</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="40" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="46" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="1">
         <v>14</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="49">
         <v>2</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="40" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>18</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="46">
         <v>8</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="40" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="46" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="1">
         <v>16</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="49">
         <v>2</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="40" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="131" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="16">
+        <v>94</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="14">
         <v>26</v>
       </c>
-      <c r="C9" s="16">
-        <v>1</v>
-      </c>
-      <c r="D9" s="54" t="s">
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="44">
+        <v>18</v>
+      </c>
+      <c r="H9" s="44">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="11"/>
+      <c r="E10" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="58">
-        <v>18</v>
-      </c>
-      <c r="H9" s="58">
-        <v>1</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="12"/>
-      <c r="E10" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="48" t="s">
-        <v>100</v>
+      <c r="J10" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -3326,61 +3296,61 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="5" max="5" width="28.36328125" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="64" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="51" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="C2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12">
+    <row r="3" spans="1:6" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="56" t="s">
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="42" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3391,16 +3361,14 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3410,7 +3378,7 @@
       <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="40" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -3418,34 +3386,32 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="59" t="s">
+    <row r="6" spans="1:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="14">
         <v>6</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="52">
         <v>8</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="40" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="12"/>
-      <c r="E7" s="53" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="11"/>
+      <c r="E7" s="39" t="s">
+        <v>103</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E8" s="1"/>
     </row>
   </sheetData>

</xml_diff>